<commit_message>
Them bản chinh sua lan 1
</commit_message>
<xml_diff>
--- a/Tổng hợp lý thuyết.xlsx
+++ b/Tổng hợp lý thuyết.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GA\Desktop\Giáo trình javascript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A9BB47-D3CC-4E32-8F4D-453E0CFF522E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A55109-52E1-4B24-93E6-F87E7D903749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9F689D61-19C6-49A7-A01D-494666BD08E5}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Một hàm không có giá trị nó sẽ là undefined</t>
   </si>
   <si>
-    <t>Khi dùng return hàm sẽ trả về giá trị dừng lại và thoát khỏi function hiện tại.</t>
-  </si>
-  <si>
     <t>Một hàm rỗng hoặc có return trống thì nó == undefined</t>
   </si>
   <si>
@@ -4493,6 +4490,9 @@
       </rPr>
       <t>))</t>
     </r>
+  </si>
+  <si>
+    <t>Khi dùng return hàm sẽ trả về giá trị, dừng lại và thoát khỏi function hiện tại.</t>
   </si>
 </sst>
 </file>
@@ -4874,9 +4874,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4888,6 +4885,9 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5208,8 +5208,8 @@
   </sheetPr>
   <dimension ref="A1:K349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O348" sqref="O348"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5220,19 +5220,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="A1" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5266,1018 +5266,1018 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
+      <c r="A11" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="33"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="37" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
-      <c r="H80" s="33"/>
-      <c r="I80" s="33"/>
-      <c r="J80" s="33"/>
-      <c r="K80" s="33"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
+      <c r="K80" s="37"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B89" s="33"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
+      <c r="A89" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="37"/>
+      <c r="C89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="37"/>
+      <c r="I89" s="37"/>
+      <c r="J89" s="37"/>
+      <c r="K89" s="37"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="33"/>
-      <c r="C104" s="33"/>
-      <c r="D104" s="33"/>
-      <c r="E104" s="33"/>
-      <c r="F104" s="33"/>
-      <c r="G104" s="33"/>
-      <c r="H104" s="33"/>
-      <c r="I104" s="33"/>
-      <c r="J104" s="33"/>
-      <c r="K104" s="33"/>
+      <c r="A104" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
+      <c r="K104" s="37"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B116" s="33"/>
-      <c r="C116" s="33"/>
-      <c r="D116" s="33"/>
-      <c r="E116" s="33"/>
-      <c r="F116" s="33"/>
-      <c r="G116" s="33"/>
-      <c r="H116" s="33"/>
-      <c r="I116" s="33"/>
-      <c r="J116" s="33"/>
-      <c r="K116" s="33"/>
+      <c r="A116" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="37"/>
+      <c r="K116" s="37"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B140" s="33"/>
-      <c r="C140" s="33"/>
-      <c r="D140" s="33"/>
-      <c r="E140" s="33"/>
-      <c r="F140" s="33"/>
-      <c r="G140" s="33"/>
-      <c r="H140" s="33"/>
-      <c r="I140" s="33"/>
-      <c r="J140" s="33"/>
-      <c r="K140" s="33"/>
+      <c r="A140" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B140" s="37"/>
+      <c r="C140" s="37"/>
+      <c r="D140" s="37"/>
+      <c r="E140" s="37"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
+      <c r="H140" s="37"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="37"/>
+      <c r="K140" s="37"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A177" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B177" s="33"/>
-      <c r="C177" s="33"/>
-      <c r="D177" s="33"/>
-      <c r="E177" s="33"/>
-      <c r="F177" s="33"/>
-      <c r="G177" s="33"/>
-      <c r="H177" s="33"/>
-      <c r="I177" s="33"/>
-      <c r="J177" s="33"/>
-      <c r="K177" s="33"/>
+      <c r="A177" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="B177" s="37"/>
+      <c r="C177" s="37"/>
+      <c r="D177" s="37"/>
+      <c r="E177" s="37"/>
+      <c r="F177" s="37"/>
+      <c r="G177" s="37"/>
+      <c r="H177" s="37"/>
+      <c r="I177" s="37"/>
+      <c r="J177" s="37"/>
+      <c r="K177" s="37"/>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
@@ -6285,202 +6285,202 @@
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A208" s="37" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A208" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="B208" s="33"/>
-      <c r="C208" s="33"/>
-      <c r="D208" s="33"/>
-      <c r="E208" s="33"/>
-      <c r="F208" s="33"/>
-      <c r="G208" s="33"/>
-      <c r="H208" s="33"/>
-      <c r="I208" s="33"/>
-      <c r="J208" s="33"/>
-      <c r="K208" s="33"/>
+      <c r="B208" s="37"/>
+      <c r="C208" s="37"/>
+      <c r="D208" s="37"/>
+      <c r="E208" s="37"/>
+      <c r="F208" s="37"/>
+      <c r="G208" s="37"/>
+      <c r="H208" s="37"/>
+      <c r="I208" s="37"/>
+      <c r="J208" s="37"/>
+      <c r="K208" s="37"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
@@ -6488,27 +6488,27 @@
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
@@ -6516,57 +6516,57 @@
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
@@ -6574,72 +6574,72 @@
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
@@ -6647,7 +6647,7 @@
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
@@ -6655,7 +6655,7 @@
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
@@ -6663,17 +6663,17 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
@@ -6681,7 +6681,7 @@
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
@@ -6689,27 +6689,27 @@
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
@@ -6717,7 +6717,7 @@
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.25">
@@ -6725,158 +6725,158 @@
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="298" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A298" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A313" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="B313" s="33"/>
-      <c r="C313" s="33"/>
-      <c r="D313" s="33"/>
-      <c r="E313" s="33"/>
-      <c r="F313" s="33"/>
-      <c r="G313" s="33"/>
-      <c r="H313" s="33"/>
-      <c r="I313" s="33"/>
-      <c r="J313" s="33"/>
-      <c r="K313" s="33"/>
+      <c r="A313" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B313" s="37"/>
+      <c r="C313" s="37"/>
+      <c r="D313" s="37"/>
+      <c r="E313" s="37"/>
+      <c r="F313" s="37"/>
+      <c r="G313" s="37"/>
+      <c r="H313" s="37"/>
+      <c r="I313" s="37"/>
+      <c r="J313" s="37"/>
+      <c r="K313" s="37"/>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
@@ -6884,133 +6884,139 @@
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" s="33" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A327" s="34" t="s">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" s="34"/>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" s="35" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A328" s="35"/>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A329" s="36" t="s">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="34"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="35" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A330" s="35"/>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A331" s="36" t="s">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="36" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A332" s="37" t="s">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="35" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A333" s="36" t="s">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="35" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A334" s="36" t="s">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" s="35" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A335" s="36" t="s">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" s="35" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A336" s="36" t="s">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="35" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="36" t="s">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="35" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="36" t="s">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="35" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="36" t="s">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="35" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="36" t="s">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="35" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="36" t="s">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="35" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="36" t="s">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="35" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="36" t="s">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="34"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="35" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="35"/>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="36" t="s">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="33" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="34" t="s">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="36" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="37" t="s">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="36" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="37" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A313:K313"/>
+    <mergeCell ref="A104:K104"/>
+    <mergeCell ref="A208:K208"/>
+    <mergeCell ref="A116:K116"/>
+    <mergeCell ref="A140:K140"/>
+    <mergeCell ref="A177:K177"/>
     <mergeCell ref="A89:K89"/>
     <mergeCell ref="A80:K80"/>
     <mergeCell ref="A1:K1"/>
@@ -7020,12 +7026,6 @@
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A45:K45"/>
     <mergeCell ref="A65:K65"/>
-    <mergeCell ref="A313:K313"/>
-    <mergeCell ref="A104:K104"/>
-    <mergeCell ref="A208:K208"/>
-    <mergeCell ref="A116:K116"/>
-    <mergeCell ref="A140:K140"/>
-    <mergeCell ref="A177:K177"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add array data type
</commit_message>
<xml_diff>
--- a/Tổng hợp lý thuyết.xlsx
+++ b/Tổng hợp lý thuyết.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GA\Desktop\Giáo trình javascript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A55109-52E1-4B24-93E6-F87E7D903749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A0C821-5589-4C08-9EAD-731E954B8E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9F689D61-19C6-49A7-A01D-494666BD08E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="302">
   <si>
     <t>Function có toàn quyền truy cập biến brên ngoài và sửa đổi nó.</t>
   </si>
@@ -541,9 +541,6 @@
   </si>
   <si>
     <t>    Vòng lặp</t>
-  </si>
-  <si>
-    <t>    Các cũ chúng ta dùng vòng lặp for(), cách mới dùng for(of);</t>
   </si>
   <si>
     <t>    [for of] chỉ cho phép truy cập vào giá trị của mảng, Không có độ dài</t>
@@ -4493,6 +4490,12 @@
   </si>
   <si>
     <t>Khi dùng return hàm sẽ trả về giá trị, dừng lại và thoát khỏi function hiện tại.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>    Cách cũ chúng ta dùng vòng lặp for(), cách mới dùng for(of);</t>
   </si>
 </sst>
 </file>
@@ -5206,10 +5209,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K349"/>
+  <dimension ref="A1:N349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O68" sqref="O68"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J195" sqref="J195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5266,7 +5269,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5654,37 +5657,40 @@
       <c r="J80" s="37"/>
       <c r="K80" s="37"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N81" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="37" t="s">
         <v>69</v>
       </c>
@@ -5699,37 +5705,37 @@
       <c r="J89" s="37"/>
       <c r="K89" s="37"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>82</v>
       </c>
@@ -6242,32 +6248,32 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>170</v>
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
@@ -6277,7 +6283,7 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
@@ -6285,32 +6291,32 @@
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B208" s="37"/>
       <c r="C208" s="37"/>
@@ -6325,17 +6331,17 @@
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
@@ -6345,37 +6351,37 @@
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
@@ -6385,7 +6391,7 @@
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
@@ -6395,17 +6401,17 @@
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
@@ -6415,27 +6421,27 @@
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
@@ -6445,42 +6451,42 @@
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
@@ -6493,22 +6499,22 @@
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
@@ -6516,17 +6522,17 @@
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
@@ -6536,37 +6542,37 @@
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
@@ -6574,67 +6580,67 @@
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
@@ -6647,7 +6653,7 @@
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
@@ -6655,7 +6661,7 @@
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
@@ -6663,17 +6669,17 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
@@ -6681,7 +6687,7 @@
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
@@ -6689,27 +6695,27 @@
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
@@ -6717,7 +6723,7 @@
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.25">
@@ -6725,108 +6731,108 @@
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="298" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A298" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B313" s="37"/>
       <c r="C313" s="37"/>
@@ -6841,42 +6847,42 @@
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
@@ -6884,25 +6890,25 @@
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -6910,7 +6916,7 @@
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -6918,67 +6924,67 @@
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="35" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="35" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
@@ -6986,17 +6992,17 @@
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
@@ -7006,17 +7012,11 @@
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A313:K313"/>
-    <mergeCell ref="A104:K104"/>
-    <mergeCell ref="A208:K208"/>
-    <mergeCell ref="A116:K116"/>
-    <mergeCell ref="A140:K140"/>
-    <mergeCell ref="A177:K177"/>
     <mergeCell ref="A89:K89"/>
     <mergeCell ref="A80:K80"/>
     <mergeCell ref="A1:K1"/>
@@ -7026,6 +7026,12 @@
     <mergeCell ref="A33:K33"/>
     <mergeCell ref="A45:K45"/>
     <mergeCell ref="A65:K65"/>
+    <mergeCell ref="A313:K313"/>
+    <mergeCell ref="A104:K104"/>
+    <mergeCell ref="A208:K208"/>
+    <mergeCell ref="A116:K116"/>
+    <mergeCell ref="A140:K140"/>
+    <mergeCell ref="A177:K177"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>